<commit_message>
Replaced an obsolete component.
</commit_message>
<xml_diff>
--- a/PCB/IBL behavior control BOM.xlsx
+++ b/PCB/IBL behavior control BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github.harp-tech\IBL_behavior_control\IBL_behavior_control\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\IBL_behavior_control\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ED0815-48A9-4326-AB7F-E7824BDCCF75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFEF50B-ACB8-4F79-8CA0-543BA1536D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ibl mainboard v1.0" sheetId="1" r:id="rId1"/>
@@ -657,12 +657,6 @@
     <t>595-SN74ACT241DW</t>
   </si>
   <si>
-    <t>M74VHC1GT126DF1G</t>
-  </si>
-  <si>
-    <t>863-M74VHC1GT126DF1G</t>
-  </si>
-  <si>
     <t>CAP CER 0603 10uF 25V ±10% X5R</t>
   </si>
   <si>
@@ -670,6 +664,12 @@
   </si>
   <si>
     <t>667-ERJ-2RKF2700X</t>
+  </si>
+  <si>
+    <t>M74VHC1GT126DT1G</t>
+  </si>
+  <si>
+    <t>863-M74VHC1GT126DT1G</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1193,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1221,15 +1221,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1599,7 +1590,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P44" sqref="P44"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,7 +1725,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>64</v>
@@ -2028,13 +2019,13 @@
       <c r="F16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I16" s="12" t="s">
+      <c r="H16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2317,7 +2308,7 @@
       <c r="G27" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="4" t="s">
         <v>62</v>
       </c>
       <c r="I27" s="9" t="s">
@@ -2341,13 +2332,13 @@
         <v>66</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>62</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -2679,13 +2670,13 @@
         <v>66</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>62</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>